<commit_message>
fixed bug in utilities.py->WriteDict_Index
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,11 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+  <si>
+    <t>INDEX</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>sib.INDEX</t>
+  </si>
+  <si>
     <t>sib.name</t>
   </si>
   <si>
@@ -28,25 +34,40 @@
     <t>sib.addr</t>
   </si>
   <si>
+    <t>frnds.INDEX</t>
+  </si>
+  <si>
     <t>frnds.b</t>
   </si>
   <si>
     <t>frnds.best</t>
   </si>
   <si>
+    <t>abhi</t>
+  </si>
+  <si>
     <t>aditi</t>
   </si>
   <si>
+    <t>ashish</t>
+  </si>
+  <si>
     <t>null</t>
   </si>
   <si>
+    <t>adadaa</t>
+  </si>
+  <si>
     <t>fjaslkff kjas</t>
   </si>
   <si>
+    <t>kjljl</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -404,13 +425,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,101 +450,328 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>98765</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
       </c>
       <c r="F2">
+        <v>2345</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>12345</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
       </c>
       <c r="F3">
+        <v>3456</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
-        <v>5</v>
+        <v>98765</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
       <c r="F7">
+        <v>12345</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
         <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>2345</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>3456</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cross product table generation
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,17 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
-  <si>
-    <t>INDEX</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>sib.INDEX</t>
-  </si>
-  <si>
     <t>sib.name</t>
   </si>
   <si>
@@ -34,9 +28,6 @@
     <t>sib.addr</t>
   </si>
   <si>
-    <t>frnds.INDEX</t>
-  </si>
-  <si>
     <t>frnds.b</t>
   </si>
   <si>
@@ -50,6 +41,27 @@
   </si>
   <si>
     <t>ashish</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
   <si>
     <t>null</t>
@@ -425,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,328 +462,741 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
+        <v>2345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>2345</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
+        <v>3456</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>3456</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>3456</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>2345</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>98765</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
+        <v>3456</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>12345</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
+        <v>2345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>3456</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>98765</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="D11">
+        <v>12345</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>2</v>
+      <c r="B12" t="s">
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>2345</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>9</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>2</v>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
+        <v>98765</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
       </c>
       <c r="F13">
-        <v>3456</v>
+        <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>12345</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="J14" t="s">
+      <c r="D16">
+        <v>98765</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
         <v>12</v>
+      </c>
+      <c r="D17">
+        <v>12345</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>98765</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>12345</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>98765</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>12345</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>98765</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <v>12345</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>2345</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>3456</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>2345</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>3456</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>2345</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>3456</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tables without parent name
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,61 +14,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>pets.name</t>
-  </si>
-  <si>
-    <t>pets.species</t>
-  </si>
-  <si>
-    <t>pets.favFoods</t>
-  </si>
-  <si>
-    <t>pets.birthYear</t>
-  </si>
-  <si>
-    <t>pets.photo</t>
-  </si>
-  <si>
-    <t>Purrsloud</t>
-  </si>
-  <si>
-    <t>Barksalot</t>
-  </si>
-  <si>
-    <t>Meowsalot</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>Dog</t>
-  </si>
-  <si>
-    <t>['wet food', 'dry food', '&lt;strong&gt;any&lt;/strong&gt; food']</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>accNo</t>
+  </si>
+  <si>
+    <t>addr</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>abhi</t>
+  </si>
+  <si>
+    <t>aditi</t>
+  </si>
+  <si>
+    <t>ashish</t>
+  </si>
+  <si>
+    <t>bank1</t>
+  </si>
+  <si>
+    <t>bank2</t>
+  </si>
+  <si>
+    <t>bank3</t>
+  </si>
+  <si>
+    <t>bank4</t>
+  </si>
+  <si>
+    <t>bank5</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
   <si>
     <t>null</t>
   </si>
   <si>
-    <t>['tuna', 'catnip', 'celery']</t>
-  </si>
-  <si>
-    <t>https://learnwebcode.github.io/json-example/images/cat-2.jpg</t>
-  </si>
-  <si>
-    <t>https://learnwebcode.github.io/json-example/images/dog-1.jpg</t>
-  </si>
-  <si>
-    <t>https://learnwebcode.github.io/json-example/images/cat-1.jpg</t>
+    <t>address1111</t>
+  </si>
+  <si>
+    <t>address2222</t>
+  </si>
+  <si>
+    <t>address3333</t>
+  </si>
+  <si>
+    <t>frnd1</t>
+  </si>
+  <si>
+    <t>frnd2</t>
+  </si>
+  <si>
+    <t>frnd3</t>
+  </si>
+  <si>
+    <t>frnd4</t>
+  </si>
+  <si>
+    <t>frnd5</t>
+  </si>
+  <si>
+    <t>frnd6</t>
+  </si>
+  <si>
+    <t>frnd8</t>
+  </si>
+  <si>
+    <t>frnd9</t>
+  </si>
+  <si>
+    <t>frnd10</t>
+  </si>
+  <si>
+    <t>frnd11</t>
+  </si>
+  <si>
+    <t>frnd12</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +131,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,22 +165,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,10 +487,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -465,62 +503,201 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>2016</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="D2">
+        <v>2345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>2008</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="D3">
+        <v>3456</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>98765</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>12345</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>2012</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>2345</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>3456</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
customize and preview added to all pages & some changes related to query of dataframe in preview page
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,39 +14,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>sib.name</t>
-  </si>
-  <si>
-    <t>sib.ph</t>
-  </si>
-  <si>
-    <t>sib.addr</t>
-  </si>
-  <si>
-    <t>frnds.b</t>
-  </si>
-  <si>
-    <t>frnds.best</t>
-  </si>
-  <si>
-    <t>aditi</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>fjaslkff kjas</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>squadName</t>
+  </si>
+  <si>
+    <t>homeTown</t>
+  </si>
+  <si>
+    <t>formed</t>
+  </si>
+  <si>
+    <t>secretBase</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>members.name</t>
+  </si>
+  <si>
+    <t>members.age</t>
+  </si>
+  <si>
+    <t>members.secretIdentity</t>
+  </si>
+  <si>
+    <t>members.powers</t>
+  </si>
+  <si>
+    <t>Super hero squad</t>
+  </si>
+  <si>
+    <t>Metro City</t>
+  </si>
+  <si>
+    <t>Super tower</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Molecule Man</t>
+  </si>
+  <si>
+    <t>Madame Uppercut</t>
+  </si>
+  <si>
+    <t>Eternal Flame</t>
+  </si>
+  <si>
+    <t>Dan Jukes</t>
+  </si>
+  <si>
+    <t>Jane Wilson</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>['Radiation resistance', 'Turning tiny', 'Radiation blast']</t>
+  </si>
+  <si>
+    <t>['Million tonne punch', 'Damage resistance', 'Superhuman reflexes']</t>
+  </si>
+  <si>
+    <t>['Immortality', 'Heat Immunity', 'Inferno', 'Teleportation', 'Interdimensional travel']</t>
   </si>
 </sst>
 </file>
@@ -404,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,101 +462,80 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>98765</v>
+        <v>2016</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>12345</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
       <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>1000000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working navbar, styling of customizaton page and selected value in preview page
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,72 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>squadName</t>
-  </si>
-  <si>
-    <t>homeTown</t>
-  </si>
-  <si>
-    <t>formed</t>
-  </si>
-  <si>
-    <t>secretBase</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>members.name</t>
-  </si>
-  <si>
-    <t>members.age</t>
-  </si>
-  <si>
-    <t>members.secretIdentity</t>
-  </si>
-  <si>
-    <t>members.powers</t>
-  </si>
-  <si>
-    <t>Super hero squad</t>
-  </si>
-  <si>
-    <t>Metro City</t>
-  </si>
-  <si>
-    <t>Super tower</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Molecule Man</t>
-  </si>
-  <si>
-    <t>Madame Uppercut</t>
-  </si>
-  <si>
-    <t>Eternal Flame</t>
-  </si>
-  <si>
-    <t>Dan Jukes</t>
-  </si>
-  <si>
-    <t>Jane Wilson</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>['Radiation resistance', 'Turning tiny', 'Radiation blast']</t>
-  </si>
-  <si>
-    <t>['Million tonne punch', 'Damage resistance', 'Superhuman reflexes']</t>
-  </si>
-  <si>
-    <t>['Immortality', 'Heat Immunity', 'Inferno', 'Teleportation', 'Interdimensional travel']</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sib.name</t>
+  </si>
+  <si>
+    <t>sib.ph</t>
+  </si>
+  <si>
+    <t>sib.addr</t>
+  </si>
+  <si>
+    <t>frnds.b</t>
+  </si>
+  <si>
+    <t>frnds.best</t>
+  </si>
+  <si>
+    <t>aditi</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>fjaslkff kjas</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -437,13 +404,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,80 +429,101 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>98765</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>2016</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>12345</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
       <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>39</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
       <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4">
-        <v>1000000</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update query backend to perform query on DF instead of PreviewDF
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -19,19 +19,19 @@
     <t>name</t>
   </si>
   <si>
-    <t>details.bank</t>
-  </si>
-  <si>
-    <t>details.accNo</t>
-  </si>
-  <si>
-    <t>details.addr</t>
-  </si>
-  <si>
-    <t>frnds.name</t>
-  </si>
-  <si>
-    <t>frnds.best</t>
+    <t>details_bank</t>
+  </si>
+  <si>
+    <t>details_accNo</t>
+  </si>
+  <si>
+    <t>details_addr</t>
+  </si>
+  <si>
+    <t>frnds_name</t>
+  </si>
+  <si>
+    <t>frnds_best</t>
   </si>
   <si>
     <t>abhi</t>

</xml_diff>

<commit_message>
add backend+frontend to download preview data
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>aditi</t>
   </si>
   <si>
-    <t>ashish</t>
-  </si>
-  <si>
     <t>bank1</t>
   </si>
   <si>
@@ -58,12 +55,6 @@
     <t>bank5</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>address2222</t>
   </si>
   <si>
-    <t>address3333</t>
-  </si>
-  <si>
     <t>frnd1</t>
   </si>
   <si>
@@ -101,12 +89,6 @@
   </si>
   <si>
     <t>frnd10</t>
-  </si>
-  <si>
-    <t>frnd11</t>
-  </si>
-  <si>
-    <t>frnd12</t>
   </si>
   <si>
     <t>false</t>
@@ -470,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,61 +486,88 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2345</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>3456</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>3456</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -566,84 +575,114 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>98765</v>
+        <v>2345</v>
       </c>
       <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>12345</v>
+        <v>3456</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2345</v>
       </c>
       <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>3456</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>98765</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -651,53 +690,321 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>2345</v>
+        <v>12345</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="D12">
-        <v>3456</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>98765</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>12345</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>98765</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>12345</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
         <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>98765</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>12345</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>98765</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>12345</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing imports in preview.js
</commit_message>
<xml_diff>
--- a/backend/generatedXlsxFile.xlsx
+++ b/backend/generatedXlsxFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -34,64 +34,31 @@
     <t>frnds_best</t>
   </si>
   <si>
-    <t>abhi</t>
-  </si>
-  <si>
     <t>aditi</t>
   </si>
   <si>
-    <t>bank1</t>
-  </si>
-  <si>
-    <t>bank2</t>
+    <t>bank5</t>
   </si>
   <si>
     <t>bank3</t>
   </si>
   <si>
-    <t>bank4</t>
-  </si>
-  <si>
-    <t>bank5</t>
-  </si>
-  <si>
     <t>null</t>
   </si>
   <si>
-    <t>address1111</t>
-  </si>
-  <si>
     <t>address2222</t>
   </si>
   <si>
-    <t>frnd1</t>
-  </si>
-  <si>
-    <t>frnd2</t>
-  </si>
-  <si>
-    <t>frnd3</t>
-  </si>
-  <si>
-    <t>frnd4</t>
-  </si>
-  <si>
-    <t>frnd5</t>
+    <t>frnd8</t>
+  </si>
+  <si>
+    <t>frnd9</t>
   </si>
   <si>
     <t>frnd6</t>
   </si>
   <si>
-    <t>frnd8</t>
-  </si>
-  <si>
-    <t>frnd9</t>
-  </si>
-  <si>
     <t>frnd10</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>true</t>
@@ -452,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,53 +447,53 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>2345</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>3456</v>
+        <v>98765</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -535,44 +502,44 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>2345</v>
+        <v>98765</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>3456</v>
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -581,44 +548,44 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>2345</v>
+        <v>98765</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>3456</v>
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -627,384 +594,39 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>2345</v>
+        <v>98765</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>3456</v>
+      <c r="D9" t="s">
+        <v>9</v>
       </c>
       <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
       <c r="G9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>98765</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>12345</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>98765</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14">
-        <v>12345</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>98765</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <v>12345</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>98765</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20">
-        <v>12345</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>98765</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23">
-        <v>12345</v>
-      </c>
-      <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>